<commit_message>
Refactored the whole project, giving it a more professional look. Also included all the essential files for deployment
</commit_message>
<xml_diff>
--- a/financial_files/excel/ANSS.xlsx
+++ b/financial_files/excel/ANSS.xlsx
@@ -8,6 +8,8 @@
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="financial_data_scraped" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="financial_statement_api" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="rule1_results" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -156,6 +158,47 @@
     <tableColumn id="13" name="2018"/>
     <tableColumn id="14" name="2019"/>
     <tableColumn id="15" name="TTM"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="financial_statement_api" displayName="financial_statement_api" ref="A1:U23" headerRowCount="1">
+  <autoFilter ref="A1:U23"/>
+  <tableColumns count="21">
+    <tableColumn id="1" name="API Parameter"/>
+    <tableColumn id="2" name="2000"/>
+    <tableColumn id="3" name="2001"/>
+    <tableColumn id="4" name="2002"/>
+    <tableColumn id="5" name="2003"/>
+    <tableColumn id="6" name="2004"/>
+    <tableColumn id="7" name="2005"/>
+    <tableColumn id="8" name="2006"/>
+    <tableColumn id="9" name="2007"/>
+    <tableColumn id="10" name="2008"/>
+    <tableColumn id="11" name="2009"/>
+    <tableColumn id="12" name="2010"/>
+    <tableColumn id="13" name="2011"/>
+    <tableColumn id="14" name="2012"/>
+    <tableColumn id="15" name="2013"/>
+    <tableColumn id="16" name="2014"/>
+    <tableColumn id="17" name="2015"/>
+    <tableColumn id="18" name="2016"/>
+    <tableColumn id="19" name="2017"/>
+    <tableColumn id="20" name="2018"/>
+    <tableColumn id="21" name="2019"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="rule1_results" displayName="rule1_results" ref="A1:B54" headerRowCount="1">
+  <autoFilter ref="A1:B54"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="Rule #1 Metric"/>
+    <tableColumn id="2" name="Value"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6826,4 +6869,2245 @@
     <tablePart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:U23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>API Parameter</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>2000</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>2001</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>2002</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>2003</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>2004</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>2005</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>2006</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>2007</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>2008</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>2009</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>2010</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>2011</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>2012</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>2013</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>2014</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>2015</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>2016</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>2017</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>revenue</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>74467000</v>
+      </c>
+      <c r="C2" t="n">
+        <v>84836000</v>
+      </c>
+      <c r="D2" t="n">
+        <v>91011000</v>
+      </c>
+      <c r="E2" t="n">
+        <v>113535000</v>
+      </c>
+      <c r="F2" t="n">
+        <v>134539000</v>
+      </c>
+      <c r="G2" t="n">
+        <v>158036000</v>
+      </c>
+      <c r="H2" t="n">
+        <v>263640000</v>
+      </c>
+      <c r="I2" t="n">
+        <v>385340000</v>
+      </c>
+      <c r="J2" t="n">
+        <v>478339000</v>
+      </c>
+      <c r="K2" t="n">
+        <v>516885000</v>
+      </c>
+      <c r="L2" t="n">
+        <v>580236000</v>
+      </c>
+      <c r="M2" t="n">
+        <v>691449000</v>
+      </c>
+      <c r="N2" t="n">
+        <v>798018000</v>
+      </c>
+      <c r="O2" t="n">
+        <v>861260000</v>
+      </c>
+      <c r="P2" t="n">
+        <v>936021000</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>942753000</v>
+      </c>
+      <c r="R2" t="n">
+        <v>988465000</v>
+      </c>
+      <c r="S2" t="n">
+        <v>1095250000</v>
+      </c>
+      <c r="T2" t="n">
+        <v>1293636000</v>
+      </c>
+      <c r="U2" t="n">
+        <v>1515892000</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>operating_income</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>19579000</v>
+      </c>
+      <c r="C3" t="n">
+        <v>18548000</v>
+      </c>
+      <c r="D3" t="n">
+        <v>27074000</v>
+      </c>
+      <c r="E3" t="n">
+        <v>33345000</v>
+      </c>
+      <c r="F3" t="n">
+        <v>29008000</v>
+      </c>
+      <c r="G3" t="n">
+        <v>58840000</v>
+      </c>
+      <c r="H3" t="n">
+        <v>64256000</v>
+      </c>
+      <c r="I3" t="n">
+        <v>126769000</v>
+      </c>
+      <c r="J3" t="n">
+        <v>169731000</v>
+      </c>
+      <c r="K3" t="n">
+        <v>186203000</v>
+      </c>
+      <c r="L3" t="n">
+        <v>219268000</v>
+      </c>
+      <c r="M3" t="n">
+        <v>265559000</v>
+      </c>
+      <c r="N3" t="n">
+        <v>294253000</v>
+      </c>
+      <c r="O3" t="n">
+        <v>321863000</v>
+      </c>
+      <c r="P3" t="n">
+        <v>347450000</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>353679000</v>
+      </c>
+      <c r="R3" t="n">
+        <v>376242000</v>
+      </c>
+      <c r="S3" t="n">
+        <v>390728000</v>
+      </c>
+      <c r="T3" t="n">
+        <v>476574000</v>
+      </c>
+      <c r="U3" t="n">
+        <v>515040000</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>pretax_income</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>23158000</v>
+      </c>
+      <c r="C4" t="n">
+        <v>19982000</v>
+      </c>
+      <c r="D4" t="n">
+        <v>27385000</v>
+      </c>
+      <c r="E4" t="n">
+        <v>30674000</v>
+      </c>
+      <c r="F4" t="n">
+        <v>47901000</v>
+      </c>
+      <c r="G4" t="n">
+        <v>63111000</v>
+      </c>
+      <c r="H4" t="n">
+        <v>33061000</v>
+      </c>
+      <c r="I4" t="n">
+        <v>124263000</v>
+      </c>
+      <c r="J4" t="n">
+        <v>166691000</v>
+      </c>
+      <c r="K4" t="n">
+        <v>173529000</v>
+      </c>
+      <c r="L4" t="n">
+        <v>216394000</v>
+      </c>
+      <c r="M4" t="n">
+        <v>264858000</v>
+      </c>
+      <c r="N4" t="n">
+        <v>293547000</v>
+      </c>
+      <c r="O4" t="n">
+        <v>322489000</v>
+      </c>
+      <c r="P4" t="n">
+        <v>348139000</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>356765000</v>
+      </c>
+      <c r="R4" t="n">
+        <v>380315000</v>
+      </c>
+      <c r="S4" t="n">
+        <v>395694000</v>
+      </c>
+      <c r="T4" t="n">
+        <v>487085000</v>
+      </c>
+      <c r="U4" t="n">
+        <v>522583000</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>income_tax</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>-6848000</v>
+      </c>
+      <c r="C5" t="n">
+        <v>-6290000</v>
+      </c>
+      <c r="D5" t="n">
+        <v>-8426000</v>
+      </c>
+      <c r="E5" t="n">
+        <v>-9361000</v>
+      </c>
+      <c r="F5" t="n">
+        <v>-13334000</v>
+      </c>
+      <c r="G5" t="n">
+        <v>-19208000</v>
+      </c>
+      <c r="H5" t="n">
+        <v>-18905000</v>
+      </c>
+      <c r="I5" t="n">
+        <v>-41871000</v>
+      </c>
+      <c r="J5" t="n">
+        <v>-55020000</v>
+      </c>
+      <c r="K5" t="n">
+        <v>-57138000</v>
+      </c>
+      <c r="L5" t="n">
+        <v>-63262000</v>
+      </c>
+      <c r="M5" t="n">
+        <v>-84183000</v>
+      </c>
+      <c r="N5" t="n">
+        <v>-90064000</v>
+      </c>
+      <c r="O5" t="n">
+        <v>-77162000</v>
+      </c>
+      <c r="P5" t="n">
+        <v>-93449000</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>-104244000</v>
+      </c>
+      <c r="R5" t="n">
+        <v>-114679000</v>
+      </c>
+      <c r="S5" t="n">
+        <v>-136443000</v>
+      </c>
+      <c r="T5" t="n">
+        <v>-67710000</v>
+      </c>
+      <c r="U5" t="n">
+        <v>-71288000</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>eps_diluted</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.22</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.52</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0.19</v>
+      </c>
+      <c r="I6" t="n">
+        <v>1.02</v>
+      </c>
+      <c r="J6" t="n">
+        <v>1.29</v>
+      </c>
+      <c r="K6" t="n">
+        <v>1.27</v>
+      </c>
+      <c r="L6" t="n">
+        <v>1.64</v>
+      </c>
+      <c r="M6" t="n">
+        <v>1.91</v>
+      </c>
+      <c r="N6" t="n">
+        <v>2.14</v>
+      </c>
+      <c r="O6" t="n">
+        <v>2.58</v>
+      </c>
+      <c r="P6" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>2.76</v>
+      </c>
+      <c r="R6" t="n">
+        <v>2.99</v>
+      </c>
+      <c r="S6" t="n">
+        <v>2.98</v>
+      </c>
+      <c r="T6" t="n">
+        <v>4.88</v>
+      </c>
+      <c r="U6" t="n">
+        <v>5.25</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>shares_diluted</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>65076000</v>
+      </c>
+      <c r="C7" t="n">
+        <v>61752000</v>
+      </c>
+      <c r="D7" t="n">
+        <v>62376000</v>
+      </c>
+      <c r="E7" t="n">
+        <v>63752000</v>
+      </c>
+      <c r="F7" t="n">
+        <v>65956000</v>
+      </c>
+      <c r="G7" t="n">
+        <v>67384000</v>
+      </c>
+      <c r="H7" t="n">
+        <v>76398000</v>
+      </c>
+      <c r="I7" t="n">
+        <v>81135000</v>
+      </c>
+      <c r="J7" t="n">
+        <v>86768000</v>
+      </c>
+      <c r="K7" t="n">
+        <v>91785000</v>
+      </c>
+      <c r="L7" t="n">
+        <v>93209000</v>
+      </c>
+      <c r="M7" t="n">
+        <v>94381000</v>
+      </c>
+      <c r="N7" t="n">
+        <v>94954000</v>
+      </c>
+      <c r="O7" t="n">
+        <v>95139000</v>
+      </c>
+      <c r="P7" t="n">
+        <v>94194000</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>91502000</v>
+      </c>
+      <c r="R7" t="n">
+        <v>88969000</v>
+      </c>
+      <c r="S7" t="n">
+        <v>86854000</v>
+      </c>
+      <c r="T7" t="n">
+        <v>85913000</v>
+      </c>
+      <c r="U7" t="n">
+        <v>85925000</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>total_assets</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>101120000</v>
+      </c>
+      <c r="C8" t="n">
+        <v>117762000</v>
+      </c>
+      <c r="D8" t="n">
+        <v>127001000</v>
+      </c>
+      <c r="E8" t="n">
+        <v>180559000</v>
+      </c>
+      <c r="F8" t="n">
+        <v>239646000</v>
+      </c>
+      <c r="G8" t="n">
+        <v>305509000</v>
+      </c>
+      <c r="H8" t="n">
+        <v>902696000</v>
+      </c>
+      <c r="I8" t="n">
+        <v>969292000</v>
+      </c>
+      <c r="J8" t="n">
+        <v>1864514000</v>
+      </c>
+      <c r="K8" t="n">
+        <v>1920182000</v>
+      </c>
+      <c r="L8" t="n">
+        <v>2126876000</v>
+      </c>
+      <c r="M8" t="n">
+        <v>2448470000</v>
+      </c>
+      <c r="N8" t="n">
+        <v>2607417000</v>
+      </c>
+      <c r="O8" t="n">
+        <v>2722382000</v>
+      </c>
+      <c r="P8" t="n">
+        <v>2752879000</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>2729904000</v>
+      </c>
+      <c r="R8" t="n">
+        <v>2800526000</v>
+      </c>
+      <c r="S8" t="n">
+        <v>2941623000</v>
+      </c>
+      <c r="T8" t="n">
+        <v>3265964000</v>
+      </c>
+      <c r="U8" t="n">
+        <v>4838887000</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>st_debt</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>0</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" t="n">
+        <v>13927000</v>
+      </c>
+      <c r="I9" t="n">
+        <v>7716000</v>
+      </c>
+      <c r="J9" t="n">
+        <v>29630000</v>
+      </c>
+      <c r="K9" t="n">
+        <v>26758000</v>
+      </c>
+      <c r="L9" t="n">
+        <v>31962000</v>
+      </c>
+      <c r="M9" t="n">
+        <v>74423000</v>
+      </c>
+      <c r="N9" t="n">
+        <v>53149000</v>
+      </c>
+      <c r="O9" t="n">
+        <v>0</v>
+      </c>
+      <c r="P9" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>0</v>
+      </c>
+      <c r="R9" t="n">
+        <v>0</v>
+      </c>
+      <c r="S9" t="n">
+        <v>0</v>
+      </c>
+      <c r="T9" t="n">
+        <v>0</v>
+      </c>
+      <c r="U9" t="n">
+        <v>75000000</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>lt_debt</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" t="n">
+        <v>109393000</v>
+      </c>
+      <c r="I10" t="n">
+        <v>52430000</v>
+      </c>
+      <c r="J10" t="n">
+        <v>249795000</v>
+      </c>
+      <c r="K10" t="n">
+        <v>198668000</v>
+      </c>
+      <c r="L10" t="n">
+        <v>127563000</v>
+      </c>
+      <c r="M10" t="n">
+        <v>53149000</v>
+      </c>
+      <c r="N10" t="n">
+        <v>0</v>
+      </c>
+      <c r="O10" t="n">
+        <v>0</v>
+      </c>
+      <c r="P10" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>0</v>
+      </c>
+      <c r="R10" t="n">
+        <v>0</v>
+      </c>
+      <c r="S10" t="n">
+        <v>0</v>
+      </c>
+      <c r="T10" t="n">
+        <v>0</v>
+      </c>
+      <c r="U10" t="n">
+        <v>423531000</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>total_equity</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>69364000</v>
+      </c>
+      <c r="C11" t="n">
+        <v>74393000</v>
+      </c>
+      <c r="D11" t="n">
+        <v>91393000</v>
+      </c>
+      <c r="E11" t="n">
+        <v>127074000</v>
+      </c>
+      <c r="F11" t="n">
+        <v>175469000</v>
+      </c>
+      <c r="G11" t="n">
+        <v>224977000</v>
+      </c>
+      <c r="H11" t="n">
+        <v>534793000</v>
+      </c>
+      <c r="I11" t="n">
+        <v>641210000</v>
+      </c>
+      <c r="J11" t="n">
+        <v>1182899000</v>
+      </c>
+      <c r="K11" t="n">
+        <v>1312631000</v>
+      </c>
+      <c r="L11" t="n">
+        <v>1529929000</v>
+      </c>
+      <c r="M11" t="n">
+        <v>1754473000</v>
+      </c>
+      <c r="N11" t="n">
+        <v>1940291000</v>
+      </c>
+      <c r="O11" t="n">
+        <v>2136246000</v>
+      </c>
+      <c r="P11" t="n">
+        <v>2217501000</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>2194427000</v>
+      </c>
+      <c r="R11" t="n">
+        <v>2208405000</v>
+      </c>
+      <c r="S11" t="n">
+        <v>2245831000</v>
+      </c>
+      <c r="T11" t="n">
+        <v>2649547000</v>
+      </c>
+      <c r="U11" t="n">
+        <v>3453379000</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>cf_cfo</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>22850000</v>
+      </c>
+      <c r="C12" t="n">
+        <v>23638000</v>
+      </c>
+      <c r="D12" t="n">
+        <v>22116000</v>
+      </c>
+      <c r="E12" t="n">
+        <v>38806000</v>
+      </c>
+      <c r="F12" t="n">
+        <v>51366000</v>
+      </c>
+      <c r="G12" t="n">
+        <v>67825000</v>
+      </c>
+      <c r="H12" t="n">
+        <v>89697000</v>
+      </c>
+      <c r="I12" t="n">
+        <v>127128000</v>
+      </c>
+      <c r="J12" t="n">
+        <v>196708000</v>
+      </c>
+      <c r="K12" t="n">
+        <v>173689000</v>
+      </c>
+      <c r="L12" t="n">
+        <v>166884000</v>
+      </c>
+      <c r="M12" t="n">
+        <v>307661000</v>
+      </c>
+      <c r="N12" t="n">
+        <v>298415000</v>
+      </c>
+      <c r="O12" t="n">
+        <v>332983000</v>
+      </c>
+      <c r="P12" t="n">
+        <v>385307000</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>375699000</v>
+      </c>
+      <c r="R12" t="n">
+        <v>365980000</v>
+      </c>
+      <c r="S12" t="n">
+        <v>427660000</v>
+      </c>
+      <c r="T12" t="n">
+        <v>484988000</v>
+      </c>
+      <c r="U12" t="n">
+        <v>499936000</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>cfi_ppe_net</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>-3173000</v>
+      </c>
+      <c r="C13" t="n">
+        <v>-2070000</v>
+      </c>
+      <c r="D13" t="n">
+        <v>-1612000</v>
+      </c>
+      <c r="E13" t="n">
+        <v>-2761000</v>
+      </c>
+      <c r="F13" t="n">
+        <v>-3191000</v>
+      </c>
+      <c r="G13" t="n">
+        <v>-4752000</v>
+      </c>
+      <c r="H13" t="n">
+        <v>-7843000</v>
+      </c>
+      <c r="I13" t="n">
+        <v>-10859000</v>
+      </c>
+      <c r="J13" t="n">
+        <v>-16639000</v>
+      </c>
+      <c r="K13" t="n">
+        <v>-8311000</v>
+      </c>
+      <c r="L13" t="n">
+        <v>-14260000</v>
+      </c>
+      <c r="M13" t="n">
+        <v>-22063000</v>
+      </c>
+      <c r="N13" t="n">
+        <v>-23977000</v>
+      </c>
+      <c r="O13" t="n">
+        <v>-28848000</v>
+      </c>
+      <c r="P13" t="n">
+        <v>-26023000</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>-16145000</v>
+      </c>
+      <c r="R13" t="n">
+        <v>-12443000</v>
+      </c>
+      <c r="S13" t="n">
+        <v>-19149000</v>
+      </c>
+      <c r="T13" t="n">
+        <v>-21762000</v>
+      </c>
+      <c r="U13" t="n">
+        <v>-44940000</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>roic</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>0.4559</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0.2514</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0.4164</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0.4523</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.4904</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0.6239</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0.0469</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0.1514</v>
+      </c>
+      <c r="J14" t="n">
+        <v>0.1263</v>
+      </c>
+      <c r="K14" t="n">
+        <v>0.0955</v>
+      </c>
+      <c r="L14" t="n">
+        <v>0.1265</v>
+      </c>
+      <c r="M14" t="n">
+        <v>0.1375</v>
+      </c>
+      <c r="N14" t="n">
+        <v>0.1439</v>
+      </c>
+      <c r="O14" t="n">
+        <v>0.1745</v>
+      </c>
+      <c r="P14" t="n">
+        <v>0.1804</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>0.1778</v>
+      </c>
+      <c r="R14" t="n">
+        <v>0.1899</v>
+      </c>
+      <c r="S14" t="n">
+        <v>0.1885</v>
+      </c>
+      <c r="T14" t="n">
+        <v>0.2591</v>
+      </c>
+      <c r="U14" t="n">
+        <v>0.1789</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>revenue_growth</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>0.1794</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0.1392</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0.0727</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0.2474</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.185</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0.1746</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0.6682</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0.4616</v>
+      </c>
+      <c r="J15" t="n">
+        <v>0.2413</v>
+      </c>
+      <c r="K15" t="n">
+        <v>0.0805</v>
+      </c>
+      <c r="L15" t="n">
+        <v>0.1225</v>
+      </c>
+      <c r="M15" t="n">
+        <v>0.1916</v>
+      </c>
+      <c r="N15" t="n">
+        <v>0.1541</v>
+      </c>
+      <c r="O15" t="n">
+        <v>0.07920000000000001</v>
+      </c>
+      <c r="P15" t="n">
+        <v>0.0868</v>
+      </c>
+      <c r="Q15" t="n">
+        <v>0.0071</v>
+      </c>
+      <c r="R15" t="n">
+        <v>0.0484</v>
+      </c>
+      <c r="S15" t="n">
+        <v>0.108</v>
+      </c>
+      <c r="T15" t="n">
+        <v>0.1811</v>
+      </c>
+      <c r="U15" t="n">
+        <v>0.1718</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>eps_diluted_growth</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>0.1363</v>
+      </c>
+      <c r="C16" t="n">
+        <v>-0.108</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0.3677</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0.0983</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.5671</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0.238</v>
+      </c>
+      <c r="H16" t="n">
+        <v>-0.7076</v>
+      </c>
+      <c r="I16" t="n">
+        <v>4.3684</v>
+      </c>
+      <c r="J16" t="n">
+        <v>0.2647</v>
+      </c>
+      <c r="K16" t="n">
+        <v>-0.0155</v>
+      </c>
+      <c r="L16" t="n">
+        <v>0.2913</v>
+      </c>
+      <c r="M16" t="n">
+        <v>0.1646</v>
+      </c>
+      <c r="N16" t="n">
+        <v>0.1204</v>
+      </c>
+      <c r="O16" t="n">
+        <v>0.2056</v>
+      </c>
+      <c r="P16" t="n">
+        <v>0.0465</v>
+      </c>
+      <c r="Q16" t="n">
+        <v>0.0222</v>
+      </c>
+      <c r="R16" t="n">
+        <v>0.0833</v>
+      </c>
+      <c r="S16" t="n">
+        <v>-0.0033</v>
+      </c>
+      <c r="T16" t="n">
+        <v>0.6375</v>
+      </c>
+      <c r="U16" t="n">
+        <v>0.07580000000000001</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>total_equity_growth</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>0.0568</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0.0725</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0.2285</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0.3904</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0.3808</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0.2821</v>
+      </c>
+      <c r="H17" t="n">
+        <v>1.3771</v>
+      </c>
+      <c r="I17" t="n">
+        <v>0.1989</v>
+      </c>
+      <c r="J17" t="n">
+        <v>0.8447</v>
+      </c>
+      <c r="K17" t="n">
+        <v>0.1096</v>
+      </c>
+      <c r="L17" t="n">
+        <v>0.1655</v>
+      </c>
+      <c r="M17" t="n">
+        <v>0.1467</v>
+      </c>
+      <c r="N17" t="n">
+        <v>0.1059</v>
+      </c>
+      <c r="O17" t="n">
+        <v>0.1009</v>
+      </c>
+      <c r="P17" t="n">
+        <v>0.038</v>
+      </c>
+      <c r="Q17" t="n">
+        <v>-0.0104</v>
+      </c>
+      <c r="R17" t="n">
+        <v>0.0063</v>
+      </c>
+      <c r="S17" t="n">
+        <v>0.0169</v>
+      </c>
+      <c r="T17" t="n">
+        <v>0.1797</v>
+      </c>
+      <c r="U17" t="n">
+        <v>0.3033</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>cfo_growth</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>0.2458</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0.0344</v>
+      </c>
+      <c r="D18" t="n">
+        <v>-0.0643</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0.7546</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0.3236</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0.3204</v>
+      </c>
+      <c r="H18" t="n">
+        <v>0.3224</v>
+      </c>
+      <c r="I18" t="n">
+        <v>0.4173</v>
+      </c>
+      <c r="J18" t="n">
+        <v>0.5473</v>
+      </c>
+      <c r="K18" t="n">
+        <v>-0.117</v>
+      </c>
+      <c r="L18" t="n">
+        <v>-0.0391</v>
+      </c>
+      <c r="M18" t="n">
+        <v>0.8435</v>
+      </c>
+      <c r="N18" t="n">
+        <v>-0.03</v>
+      </c>
+      <c r="O18" t="n">
+        <v>0.1158</v>
+      </c>
+      <c r="P18" t="n">
+        <v>0.1571</v>
+      </c>
+      <c r="Q18" t="n">
+        <v>-0.0249</v>
+      </c>
+      <c r="R18" t="n">
+        <v>-0.0258</v>
+      </c>
+      <c r="S18" t="n">
+        <v>0.1685</v>
+      </c>
+      <c r="T18" t="n">
+        <v>0.134</v>
+      </c>
+      <c r="U18" t="n">
+        <v>0.0308</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>fcf_growth</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>0.1865</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0.0961</v>
+      </c>
+      <c r="D19" t="n">
+        <v>-0.0493</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0.7579</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0.3365</v>
+      </c>
+      <c r="G19" t="n">
+        <v>0.3092</v>
+      </c>
+      <c r="H19" t="n">
+        <v>0.2977</v>
+      </c>
+      <c r="I19" t="n">
+        <v>0.4204</v>
+      </c>
+      <c r="J19" t="n">
+        <v>0.5487</v>
+      </c>
+      <c r="K19" t="n">
+        <v>-0.0815</v>
+      </c>
+      <c r="L19" t="n">
+        <v>-0.0771</v>
+      </c>
+      <c r="M19" t="n">
+        <v>0.8712</v>
+      </c>
+      <c r="N19" t="n">
+        <v>-0.039</v>
+      </c>
+      <c r="O19" t="n">
+        <v>0.1082</v>
+      </c>
+      <c r="P19" t="n">
+        <v>0.1813</v>
+      </c>
+      <c r="Q19" t="n">
+        <v>0.0007</v>
+      </c>
+      <c r="R19" t="n">
+        <v>-0.0167</v>
+      </c>
+      <c r="S19" t="n">
+        <v>0.1554</v>
+      </c>
+      <c r="T19" t="n">
+        <v>0.1339</v>
+      </c>
+      <c r="U19" t="n">
+        <v>-0.0177</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>fcf</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>19677000</v>
+      </c>
+      <c r="C20" t="n">
+        <v>21568000</v>
+      </c>
+      <c r="D20" t="n">
+        <v>20504000</v>
+      </c>
+      <c r="E20" t="n">
+        <v>36045000</v>
+      </c>
+      <c r="F20" t="n">
+        <v>48175000</v>
+      </c>
+      <c r="G20" t="n">
+        <v>63073000</v>
+      </c>
+      <c r="H20" t="n">
+        <v>81854000</v>
+      </c>
+      <c r="I20" t="n">
+        <v>116269000</v>
+      </c>
+      <c r="J20" t="n">
+        <v>180069000</v>
+      </c>
+      <c r="K20" t="n">
+        <v>165378000</v>
+      </c>
+      <c r="L20" t="n">
+        <v>152624000</v>
+      </c>
+      <c r="M20" t="n">
+        <v>285598000</v>
+      </c>
+      <c r="N20" t="n">
+        <v>274438000</v>
+      </c>
+      <c r="O20" t="n">
+        <v>304135000</v>
+      </c>
+      <c r="P20" t="n">
+        <v>359284000</v>
+      </c>
+      <c r="Q20" t="n">
+        <v>359554000</v>
+      </c>
+      <c r="R20" t="n">
+        <v>353537000</v>
+      </c>
+      <c r="S20" t="n">
+        <v>408511000</v>
+      </c>
+      <c r="T20" t="n">
+        <v>463226000</v>
+      </c>
+      <c r="U20" t="n">
+        <v>454996000</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>book_value_per_share</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>1.0658</v>
+      </c>
+      <c r="C21" t="n">
+        <v>1.2047</v>
+      </c>
+      <c r="D21" t="n">
+        <v>1.4651</v>
+      </c>
+      <c r="E21" t="n">
+        <v>1.9932</v>
+      </c>
+      <c r="F21" t="n">
+        <v>2.6603</v>
+      </c>
+      <c r="G21" t="n">
+        <v>3.3387</v>
+      </c>
+      <c r="H21" t="n">
+        <v>7</v>
+      </c>
+      <c r="I21" t="n">
+        <v>7.903</v>
+      </c>
+      <c r="J21" t="n">
+        <v>13.6328</v>
+      </c>
+      <c r="K21" t="n">
+        <v>14.3011</v>
+      </c>
+      <c r="L21" t="n">
+        <v>16.4139</v>
+      </c>
+      <c r="M21" t="n">
+        <v>18.5892</v>
+      </c>
+      <c r="N21" t="n">
+        <v>20.434</v>
+      </c>
+      <c r="O21" t="n">
+        <v>22.4539</v>
+      </c>
+      <c r="P21" t="n">
+        <v>23.5418</v>
+      </c>
+      <c r="Q21" t="n">
+        <v>23.9822</v>
+      </c>
+      <c r="R21" t="n">
+        <v>24.8221</v>
+      </c>
+      <c r="S21" t="n">
+        <v>25.8575</v>
+      </c>
+      <c r="T21" t="n">
+        <v>30.8398</v>
+      </c>
+      <c r="U21" t="n">
+        <v>40.1906</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>market_cap</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>170094920</v>
+      </c>
+      <c r="C22" t="n">
+        <v>357618800</v>
+      </c>
+      <c r="D22" t="n">
+        <v>294308950</v>
+      </c>
+      <c r="E22" t="n">
+        <v>608460750</v>
+      </c>
+      <c r="F22" t="n">
+        <v>1007196960</v>
+      </c>
+      <c r="G22" t="n">
+        <v>1368449600</v>
+      </c>
+      <c r="H22" t="n">
+        <v>1678730250</v>
+      </c>
+      <c r="I22" t="n">
+        <v>3242130540</v>
+      </c>
+      <c r="J22" t="n">
+        <v>2494537380</v>
+      </c>
+      <c r="K22" t="n">
+        <v>3897318960</v>
+      </c>
+      <c r="L22" t="n">
+        <v>4772059290</v>
+      </c>
+      <c r="M22" t="n">
+        <v>5307106560</v>
+      </c>
+      <c r="N22" t="n">
+        <v>6240128440</v>
+      </c>
+      <c r="O22" t="n">
+        <v>8050129600</v>
+      </c>
+      <c r="P22" t="n">
+        <v>7442730000</v>
+      </c>
+      <c r="Q22" t="n">
+        <v>8152950000</v>
+      </c>
+      <c r="R22" t="n">
+        <v>7925283120</v>
+      </c>
+      <c r="S22" t="n">
+        <v>12425897280</v>
+      </c>
+      <c r="T22" t="n">
+        <v>11954643960</v>
+      </c>
+      <c r="U22" t="n">
+        <v>22068788940</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>price_to_earnings</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>10.4288</v>
+      </c>
+      <c r="C23" t="n">
+        <v>26.1188</v>
+      </c>
+      <c r="D23" t="n">
+        <v>15.5234</v>
+      </c>
+      <c r="E23" t="n">
+        <v>28.5488</v>
+      </c>
+      <c r="F23" t="n">
+        <v>29.1375</v>
+      </c>
+      <c r="G23" t="n">
+        <v>31.1698</v>
+      </c>
+      <c r="H23" t="n">
+        <v>118.5878</v>
+      </c>
+      <c r="I23" t="n">
+        <v>39.35</v>
+      </c>
+      <c r="J23" t="n">
+        <v>22.3382</v>
+      </c>
+      <c r="K23" t="n">
+        <v>33.4847</v>
+      </c>
+      <c r="L23" t="n">
+        <v>31.163</v>
+      </c>
+      <c r="M23" t="n">
+        <v>29.3737</v>
+      </c>
+      <c r="N23" t="n">
+        <v>30.6665</v>
+      </c>
+      <c r="O23" t="n">
+        <v>32.8138</v>
+      </c>
+      <c r="P23" t="n">
+        <v>29.2227</v>
+      </c>
+      <c r="Q23" t="n">
+        <v>32.2862</v>
+      </c>
+      <c r="R23" t="n">
+        <v>29.8351</v>
+      </c>
+      <c r="S23" t="n">
+        <v>47.9299</v>
+      </c>
+      <c r="T23" t="n">
+        <v>28.5058</v>
+      </c>
+      <c r="U23" t="n">
+        <v>48.901</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <tableParts count="1">
+    <tablePart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B54"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Rule #1 Metric</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Value</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>ROIC - 10-year</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>11.34%</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>ROIC - 5-year</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>12.29%</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>ROIC - 3-year</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>12.71%</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>ROIC - 1-year</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>11.25%</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>ROIC QuickFS - 10-year</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>17.57%</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>ROIC QuickFS - 5-year</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>19.88%</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>ROIC QuickFS - 3-year</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>20.88%</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>ROIC QuickFS - 1-year</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>17.89%</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Equity Growth Rate - 10-year</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>10.89%</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Equity Growth Rate - 5-year</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>11.29%</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Equity Growth Rate - 3-year</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>17.43%</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Equity Growth Rate - 1-year</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>30.32%</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>EPS Growth Rate - 10-year</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>15.25%</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>EPS Growth Rate - 5-year</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>14.22%</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>EPS Growth Rate - 3-year</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>20.64%</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>EPS Growth Rate - 1-year</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>7.58%</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Sales Growth Rate - 10-year</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>11.36%</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Sales Growth Rate - 5-year</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>10.12%</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Sales Growth Rate - 3-year</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>15.32%</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Sales Growth Rate - 1-year</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>17.18%</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>FCF Growth Rate - 10-year</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>10.65%</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>FCF Growth Rate - 5-year</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>4.84%</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>FCF Growth Rate - 3-year</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>8.77%</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>FCF Growth Rate - 1-year</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>-1.78%</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>OCF Growth Rate - 10-year</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>11.15%</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>OCF Growth Rate - 5-year</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>5.35%</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>OCF Growth Rate - 3-year</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>10.96%</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>OCF Growth Rate - 1-year</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>3.08%</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Debt - Current Long-Term Debt</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>423531000</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Debt - Payoff Possible</t>
+        </is>
+      </c>
+      <c r="B31" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>current_eps</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>4.399000200844951</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>analyst_growth_rate</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>0.0639</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>equity_growth_rate</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>0.1748046125720419</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>eps_growth_rate</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>0.0639</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>future_eps</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>8.172634388135146</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>average_historical_pe</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>34.06977</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>default_pe</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>12.78</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>future_pe</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>12.78</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>future_market_price</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>104.4462674803672</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>sticker_price</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>25.81751993266035</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>margin_of_safety</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>12.90875996633017</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>shortName</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>ANSYS, Inc.</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>symbol</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>ANSS</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>currency</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>country</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>market</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>us_market</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>exchange</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>NMS</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>sector</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Technology</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>industry</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Software—Application</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>website</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>http://www.ansys.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>marketCap</t>
+        </is>
+      </c>
+      <c r="B52" t="n">
+        <v>31244632064</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>volume</t>
+        </is>
+      </c>
+      <c r="B53" t="n">
+        <v>367643</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>forwardPE</t>
+        </is>
+      </c>
+      <c r="B54" t="n">
+        <v>51.602833</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <tableParts count="1">
+    <tablePart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>